<commit_message>
Updated Gantt chart for JUnit
</commit_message>
<xml_diff>
--- a/Phase 3 Documents/Gantt Chart - Updated P3.xlsx
+++ b/Phase 3 Documents/Gantt Chart - Updated P3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\communicationsGroup4\Phase 3 Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/Documents/GitHub/communicationsGroup4/Phase 3 Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E93F5E9-E72B-481E-A340-7F1B682277E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35867FDB-F966-3C42-91EC-44D76FB1742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>Development</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>3. Outer Client Side Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a. Unit Testing</t>
   </si>
 </sst>
 </file>
@@ -666,7 +669,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N44" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N47" headerRowDxfId="0">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Development"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assigned to"/>
@@ -888,24 +891,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -949,7 +952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -989,13 +992,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1006,7 +1009,7 @@
       </c>
       <c r="N4" s="23"/>
     </row>
-    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1018,7 +1021,7 @@
       <c r="E5" s="15"/>
       <c r="N5" s="23"/>
     </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1030,7 +1033,7 @@
       <c r="E6" s="15"/>
       <c r="N6" s="23"/>
     </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1042,7 +1045,7 @@
       <c r="E7" s="15"/>
       <c r="N7" s="23"/>
     </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1054,7 +1057,7 @@
       <c r="E8" s="15"/>
       <c r="N8" s="23"/>
     </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -1066,7 +1069,7 @@
       <c r="E9" s="15"/>
       <c r="N9" s="23"/>
     </row>
-    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1078,7 +1081,7 @@
       <c r="E10" s="15"/>
       <c r="N10" s="23"/>
     </row>
-    <row r="11" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1090,7 +1093,7 @@
       <c r="E11" s="15"/>
       <c r="N11" s="23"/>
     </row>
-    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -1102,7 +1105,7 @@
       <c r="E12" s="15"/>
       <c r="N12" s="23"/>
     </row>
-    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -1114,7 +1117,7 @@
       <c r="E13" s="24"/>
       <c r="N13" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1123,17 +1126,17 @@
       </c>
       <c r="N14" s="23"/>
     </row>
-    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="N15" s="23"/>
     </row>
-    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
       <c r="N16" s="23"/>
     </row>
-    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
@@ -1146,7 +1149,7 @@
       </c>
       <c r="N17" s="23"/>
     </row>
-    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
         <v>57</v>
       </c>
@@ -1159,7 +1162,7 @@
       <c r="G18" s="26"/>
       <c r="N18" s="23"/>
     </row>
-    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="27" t="s">
         <v>58</v>
       </c>
@@ -1173,7 +1176,7 @@
       <c r="J19" s="15"/>
       <c r="N19" s="23"/>
     </row>
-    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="27" t="s">
         <v>59</v>
       </c>
@@ -1187,7 +1190,7 @@
       <c r="J20" s="15"/>
       <c r="N20" s="23"/>
     </row>
-    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="27" t="s">
         <v>60</v>
       </c>
@@ -1200,7 +1203,7 @@
       <c r="J21" s="15"/>
       <c r="N21" s="23"/>
     </row>
-    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>49</v>
       </c>
@@ -1214,7 +1217,7 @@
       <c r="J22" s="15"/>
       <c r="N22" s="23"/>
     </row>
-    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>50</v>
       </c>
@@ -1228,7 +1231,7 @@
       <c r="J23" s="15"/>
       <c r="N23" s="23"/>
     </row>
-    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
         <v>61</v>
       </c>
@@ -1239,7 +1242,7 @@
       <c r="J24" s="15"/>
       <c r="N24" s="23"/>
     </row>
-    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>51</v>
       </c>
@@ -1253,7 +1256,7 @@
       <c r="J25" s="15"/>
       <c r="N25" s="23"/>
     </row>
-    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>52</v>
       </c>
@@ -1267,7 +1270,7 @@
       <c r="J26" s="15"/>
       <c r="N26" s="23"/>
     </row>
-    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
@@ -1278,7 +1281,7 @@
       <c r="J27" s="15"/>
       <c r="N27" s="23"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
@@ -1287,17 +1290,17 @@
       </c>
       <c r="N28" s="23"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9"/>
       <c r="N29" s="23"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
         <v>63</v>
       </c>
       <c r="N30" s="23"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>64</v>
       </c>
@@ -1322,25 +1325,22 @@
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="15"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="29"/>
@@ -1348,59 +1348,92 @@
       <c r="M34" s="29"/>
       <c r="N34" s="29"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" s="15"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="N38" s="23"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="5"/>
+      <c r="N41" s="23"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N39" s="25" t="s">
+      <c r="N42" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N40" s="25" t="s">
+      <c r="N43" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N41" s="23"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N42" s="23"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N43" s="23"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="N44" s="20"/>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N44" s="23"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N45" s="23"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N46" s="23"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="8"/>
+      <c r="N47" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to include Docmentation
Added Risk Management Plan and Unit Test Document.
</commit_message>
<xml_diff>
--- a/Phase 3 Documents/Gantt Chart - Updated P3.xlsx
+++ b/Phase 3 Documents/Gantt Chart - Updated P3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/Documents/GitHub/communicationsGroup4/Phase 3 Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35867FDB-F966-3C42-91EC-44D76FB1742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0456B06F-FCA7-764C-9374-2BBCD2F5FEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t>Development</t>
   </si>
@@ -208,9 +208,6 @@
     <t>5. Prototype</t>
   </si>
   <si>
-    <t>5/8 (Thursday)</t>
-  </si>
-  <si>
     <t>Phase 3</t>
   </si>
   <si>
@@ -224,6 +221,18 @@
   </si>
   <si>
     <t xml:space="preserve">    a. Unit Testing</t>
+  </si>
+  <si>
+    <t>5/6 (Tuesday)</t>
+  </si>
+  <si>
+    <t>5/6 - 5/8</t>
+  </si>
+  <si>
+    <t>Risk Management Plan</t>
+  </si>
+  <si>
+    <t>Unit Test Documentation</t>
   </si>
 </sst>
 </file>
@@ -241,6 +250,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,6 +258,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -527,7 +538,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -610,6 +621,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
@@ -669,7 +681,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N47" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N49" headerRowDxfId="0">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Development"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assigned to"/>
@@ -891,11 +903,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1296,7 +1308,7 @@
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N30" s="23"/>
     </row>
@@ -1309,12 +1321,12 @@
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
       <c r="N31" s="25" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
@@ -1327,7 +1339,7 @@
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>37</v>
@@ -1337,7 +1349,7 @@
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -1350,7 +1362,7 @@
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>29</v>
@@ -1360,7 +1372,7 @@
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
@@ -1373,7 +1385,7 @@
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>31</v>
@@ -1382,58 +1394,82 @@
       <c r="N37" s="29"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="9"/>
+      <c r="A38" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-    </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="5"/>
-      <c r="N41" s="23"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="5"/>
+      <c r="N43" s="23"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N42" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
+      <c r="N44" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N43" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N44" s="23"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N45" s="23"/>
+      <c r="N45" s="25" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N46" s="23"/>
     </row>
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="8"/>
-      <c r="N47" s="20"/>
+      <c r="N47" s="23"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N48" s="23"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="8"/>
+      <c r="N49" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Gantt Chart to include Documents to work on
</commit_message>
<xml_diff>
--- a/Phase 3 Documents/Gantt Chart - Updated P3.xlsx
+++ b/Phase 3 Documents/Gantt Chart - Updated P3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/Documents/GitHub/communicationsGroup4/Phase 3 Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\communicationsGroup4\Phase 3 Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0456B06F-FCA7-764C-9374-2BBCD2F5FEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DBE0A8-5CB0-47EF-ADFA-8A20BB32E906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>Development</t>
   </si>
@@ -211,15 +211,6 @@
     <t>Phase 3</t>
   </si>
   <si>
-    <t>1. Server Side Code</t>
-  </si>
-  <si>
-    <t>2. Inner Client Side Code</t>
-  </si>
-  <si>
-    <t>3. Outer Client Side Code</t>
-  </si>
-  <si>
     <t xml:space="preserve">    a. Unit Testing</t>
   </si>
   <si>
@@ -229,17 +220,32 @@
     <t>5/6 - 5/8</t>
   </si>
   <si>
-    <t>Risk Management Plan</t>
-  </si>
-  <si>
     <t>Unit Test Documentation</t>
+  </si>
+  <si>
+    <t>Risk Management Plan*</t>
+  </si>
+  <si>
+    <t>Style Guide Documentation*</t>
+  </si>
+  <si>
+    <t>1. Server Side Code / Server, DBManager…</t>
+  </si>
+  <si>
+    <t>2. Inner Client Side Code / Chat, Message, User</t>
+  </si>
+  <si>
+    <t>3. Outer Client Side Code / Client, GUI</t>
+  </si>
+  <si>
+    <t>*Optional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -312,6 +318,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -538,7 +552,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -622,6 +636,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
@@ -681,7 +699,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N49" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N51" headerRowDxfId="0">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Development"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assigned to"/>
@@ -903,24 +921,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -964,7 +982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -1004,13 +1022,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1039,7 @@
       </c>
       <c r="N4" s="23"/>
     </row>
-    <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1051,7 @@
       <c r="E5" s="15"/>
       <c r="N5" s="23"/>
     </row>
-    <row r="6" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1045,7 +1063,7 @@
       <c r="E6" s="15"/>
       <c r="N6" s="23"/>
     </row>
-    <row r="7" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1057,7 +1075,7 @@
       <c r="E7" s="15"/>
       <c r="N7" s="23"/>
     </row>
-    <row r="8" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1069,7 +1087,7 @@
       <c r="E8" s="15"/>
       <c r="N8" s="23"/>
     </row>
-    <row r="9" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -1081,7 +1099,7 @@
       <c r="E9" s="15"/>
       <c r="N9" s="23"/>
     </row>
-    <row r="10" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1093,7 +1111,7 @@
       <c r="E10" s="15"/>
       <c r="N10" s="23"/>
     </row>
-    <row r="11" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1105,7 +1123,7 @@
       <c r="E11" s="15"/>
       <c r="N11" s="23"/>
     </row>
-    <row r="12" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -1117,7 +1135,7 @@
       <c r="E12" s="15"/>
       <c r="N12" s="23"/>
     </row>
-    <row r="13" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
@@ -1129,7 +1147,7 @@
       <c r="E13" s="24"/>
       <c r="N13" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1138,17 +1156,17 @@
       </c>
       <c r="N14" s="23"/>
     </row>
-    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="N15" s="23"/>
     </row>
-    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>42</v>
       </c>
       <c r="N16" s="23"/>
     </row>
-    <row r="17" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
@@ -1161,7 +1179,7 @@
       </c>
       <c r="N17" s="23"/>
     </row>
-    <row r="18" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>57</v>
       </c>
@@ -1174,7 +1192,7 @@
       <c r="G18" s="26"/>
       <c r="N18" s="23"/>
     </row>
-    <row r="19" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>58</v>
       </c>
@@ -1188,7 +1206,7 @@
       <c r="J19" s="15"/>
       <c r="N19" s="23"/>
     </row>
-    <row r="20" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>59</v>
       </c>
@@ -1202,7 +1220,7 @@
       <c r="J20" s="15"/>
       <c r="N20" s="23"/>
     </row>
-    <row r="21" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1233,7 @@
       <c r="J21" s="15"/>
       <c r="N21" s="23"/>
     </row>
-    <row r="22" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>49</v>
       </c>
@@ -1229,7 +1247,7 @@
       <c r="J22" s="15"/>
       <c r="N22" s="23"/>
     </row>
-    <row r="23" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>50</v>
       </c>
@@ -1243,7 +1261,7 @@
       <c r="J23" s="15"/>
       <c r="N23" s="23"/>
     </row>
-    <row r="24" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
         <v>61</v>
       </c>
@@ -1254,7 +1272,7 @@
       <c r="J24" s="15"/>
       <c r="N24" s="23"/>
     </row>
-    <row r="25" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>51</v>
       </c>
@@ -1268,7 +1286,7 @@
       <c r="J25" s="15"/>
       <c r="N25" s="23"/>
     </row>
-    <row r="26" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>52</v>
       </c>
@@ -1282,7 +1300,7 @@
       <c r="J26" s="15"/>
       <c r="N26" s="23"/>
     </row>
-    <row r="27" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
@@ -1293,7 +1311,7 @@
       <c r="J27" s="15"/>
       <c r="N27" s="23"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
@@ -1302,44 +1320,44 @@
       </c>
       <c r="N28" s="23"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="N29" s="23"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>62</v>
       </c>
       <c r="N30" s="23"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J31" s="21"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
       <c r="M31" s="25"/>
       <c r="N31" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="J32" s="15"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>37</v>
@@ -1347,129 +1365,144 @@
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J34" s="15"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
       <c r="M34" s="29"/>
       <c r="N34" s="29"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M35" s="29"/>
       <c r="N35" s="29"/>
     </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J36" s="15"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
       <c r="M36" s="29"/>
       <c r="N36" s="29"/>
     </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>31</v>
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
       </c>
       <c r="M37" s="29"/>
       <c r="N37" s="29"/>
     </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
       <c r="M38" s="30"/>
       <c r="N38" s="30"/>
     </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
       <c r="M39" s="30"/>
       <c r="N39" s="30"/>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="9"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="6" t="s">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="32"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="5"/>
-      <c r="N43" s="23"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="7" t="s">
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="N45" s="23"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N44" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="6" t="s">
+      <c r="N46" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N45" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N46" s="23"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N47" s="23"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N47" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N48" s="23"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="8"/>
-      <c r="N49" s="20"/>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N49" s="23"/>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N50" s="23"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="8"/>
+      <c r="N51" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>